<commit_message>
fix bug in travel to zone sea and hell
</commit_message>
<xml_diff>
--- a/autoSave NPCs-ITEMs/NpcsAo-Web.xlsx
+++ b/autoSave NPCs-ITEMs/NpcsAo-Web.xlsx
@@ -615,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1344,10 +1344,10 @@
         <v>80</v>
       </c>
       <c r="D18" s="19">
-        <v>100</v>
+        <v>30000</v>
       </c>
       <c r="E18" s="19">
-        <v>80</v>
+        <v>20000</v>
       </c>
       <c r="F18" s="19">
         <v>170</v>
@@ -1385,10 +1385,12 @@
         <v>90</v>
       </c>
       <c r="D19" s="19">
-        <v>120</v>
+        <f>D18*2</f>
+        <v>60000</v>
       </c>
       <c r="E19" s="19">
-        <v>90</v>
+        <f>E18*2</f>
+        <v>40000</v>
       </c>
       <c r="F19" s="19">
         <v>180</v>
@@ -1426,10 +1428,12 @@
         <v>100</v>
       </c>
       <c r="D20" s="19">
-        <v>200</v>
+        <f>D19*2</f>
+        <v>120000</v>
       </c>
       <c r="E20" s="19">
-        <v>100</v>
+        <f>E19*2</f>
+        <v>80000</v>
       </c>
       <c r="F20" s="19">
         <v>190</v>

</xml_diff>